<commit_message>
Changes done. Added invalid test case
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\B98AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245EC0A8-069D-4A26-B05F-3ED36E1DA304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFF47AA-21BE-4931-A0F6-11F018EB41DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="360" windowWidth="20325" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>ADMIN</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -356,7 +363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -381,4 +388,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456D1003-8E88-4A70-8B7E-C4AE7AFD8CDE}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>